<commit_message>
Order collection api in progress
</commit_message>
<xml_diff>
--- a/tmallOrders.xlsx
+++ b/tmallOrders.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55" count="55">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77" count="77">
   <x:si>
     <x:t>created</x:t>
   </x:si>
@@ -61,124 +61,190 @@
     <x:t>orders_order_0_title</x:t>
   </x:si>
   <x:si>
-    <x:t>2018-04-11 12:44:00</x:t>
+    <x:t>2018-04-18 22:20:38</x:t>
   </x:si>
   <x:si>
     <x:t>KEYCLUE海外旗舰店</x:t>
   </x:si>
   <x:si>
-    <x:t>fspp9494</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-04-11 12:44:09</x:t>
-  </x:si>
-  <x:si>
-    <x:t>冯珊珊</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18107988175</x:t>
-  </x:si>
-  <x:si>
-    <x:t>333000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>江西省</x:t>
-  </x:si>
-  <x:si>
-    <x:t>景德镇市</x:t>
-  </x:si>
-  <x:si>
-    <x:t>珠山区</x:t>
-  </x:si>
-  <x:si>
-    <x:t>珠山街道莲花山庄人事局宿舍</x:t>
-  </x:si>
-  <x:si>
-    <x:t>S81TS05NVF</x:t>
-  </x:si>
-  <x:si>
-    <x:t>235.06</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Salad bowls官方正品春季新款 韩版圆领双色百搭短袖上衣女</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-04-11 08:46:54</x:t>
-  </x:si>
-  <x:si>
-    <x:t>明眸0717</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-04-11 08:48:42</x:t>
-  </x:si>
-  <x:si>
-    <x:t>范钦玲</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18852848298</x:t>
-  </x:si>
-  <x:si>
-    <x:t>212400</x:t>
-  </x:si>
-  <x:si>
-    <x:t>江苏省</x:t>
-  </x:si>
-  <x:si>
-    <x:t>镇江市</x:t>
-  </x:si>
-  <x:si>
-    <x:t>句容市</x:t>
-  </x:si>
-  <x:si>
-    <x:t>江苏农林职业技术学院</x:t>
-  </x:si>
-  <x:si>
-    <x:t>S72TS50NV</x:t>
-  </x:si>
-  <x:si>
-    <x:t>269.00</x:t>
+    <x:t>fancong6985</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-04-18 22:20:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>樊聪</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13811765578</x:t>
+  </x:si>
+  <x:si>
+    <x:t>100011</x:t>
+  </x:si>
+  <x:si>
+    <x:t>北京</x:t>
+  </x:si>
+  <x:si>
+    <x:t>北京市</x:t>
+  </x:si>
+  <x:si>
+    <x:t>朝阳区</x:t>
+  </x:si>
+  <x:si>
+    <x:t>奥运村街道朝阳区域清街2号院融域嘉园4号楼6单元801</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EEOG1WSR02W_YLF</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1241.04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>eyeye春季新款韩版潮流时尚V领条纹蝴蝶袖上衣T恤</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-04-18 20:44:27</x:t>
+  </x:si>
+  <x:si>
+    <x:t>郭舒君1234</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-04-18 20:44:32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>郭舒君</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13829910807</x:t>
+  </x:si>
+  <x:si>
+    <x:t>516001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>广东省</x:t>
+  </x:si>
+  <x:si>
+    <x:t>惠州市</x:t>
+  </x:si>
+  <x:si>
+    <x:t>惠城区</x:t>
+  </x:si>
+  <x:si>
+    <x:t>江北街道江北佳兆业二期A3座806房</x:t>
+  </x:si>
+  <x:si>
+    <x:t>mnmm17ssc21_7p</x:t>
+  </x:si>
+  <x:si>
+    <x:t>323.39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>MIDNIGHT MOMENT.人造珍珠链条iPhone7/6苹果手机保护壳韩国</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-04-17 22:23:42</x:t>
+  </x:si>
+  <x:si>
+    <x:t>凯凯99977573209</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-04-17 22:25:08</x:t>
+  </x:si>
+  <x:si>
+    <x:t>汪凯旋</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13640787455</x:t>
+  </x:si>
+  <x:si>
+    <x:t>510180</x:t>
+  </x:si>
+  <x:si>
+    <x:t>广州市</x:t>
+  </x:si>
+  <x:si>
+    <x:t>越秀区</x:t>
+  </x:si>
+  <x:si>
+    <x:t>珠光街道 沿江中路299号海俊酒店前台</x:t>
+  </x:si>
+  <x:si>
+    <x:t>S72BL08BK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>399.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Salad bowls官方正品韩版甜美公主风一字肩短袖韩国包邮</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-04-17 20:38:01</x:t>
+  </x:si>
+  <x:si>
+    <x:t>takigo92</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-04-17 20:38:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>楼旦韵</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13616511558</x:t>
+  </x:si>
+  <x:si>
+    <x:t>310013</x:t>
+  </x:si>
+  <x:si>
+    <x:t>浙江省</x:t>
+  </x:si>
+  <x:si>
+    <x:t>杭州市</x:t>
+  </x:si>
+  <x:si>
+    <x:t>西湖区</x:t>
+  </x:si>
+  <x:si>
+    <x:t>杭州市西湖区黄姑山路38-1号十足(菜鸟驿站:0571-88116223)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>S72TS50IV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>299.00</x:t>
   </x:si>
   <x:si>
     <x:t>Salad bowls官方正品韩版可爱清新假V领百搭短袖韩国包邮</x:t>
   </x:si>
   <x:si>
-    <x:t>2018-04-11 08:34:08</x:t>
-  </x:si>
-  <x:si>
-    <x:t>yinshi_love</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2018-04-11 08:34:20</x:t>
-  </x:si>
-  <x:si>
-    <x:t>崔银实</x:t>
-  </x:si>
-  <x:si>
-    <x:t>18844358889</x:t>
-  </x:si>
-  <x:si>
-    <x:t>133000</x:t>
-  </x:si>
-  <x:si>
-    <x:t>吉林省</x:t>
-  </x:si>
-  <x:si>
-    <x:t>延边朝鲜族自治州</x:t>
-  </x:si>
-  <x:si>
-    <x:t>延吉市</x:t>
-  </x:si>
-  <x:si>
-    <x:t>公园街道大学城5号楼4单元1101</x:t>
-  </x:si>
-  <x:si>
-    <x:t>L17SUPT04WHF</x:t>
-  </x:si>
-  <x:si>
-    <x:t>659.16</x:t>
-  </x:si>
-  <x:si>
-    <x:t>lartigent 官方正品韩版百搭时尚直筒均码休闲短裤 韩国包邮</x:t>
+    <x:t>2018-04-12 22:43:26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>missvan82</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2018-04-12 22:43:36</x:t>
+  </x:si>
+  <x:si>
+    <x:t>泛泛</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18667162213</x:t>
+  </x:si>
+  <x:si>
+    <x:t>310012</x:t>
+  </x:si>
+  <x:si>
+    <x:t>三墩镇白马尊邸11-2-301</x:t>
+  </x:si>
+  <x:si>
+    <x:t>S72TS12NV</x:t>
+  </x:si>
+  <x:si>
+    <x:t>279.00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Salad bowls官方正品韩版宽松宽条纹圆领彩色短袖韩国包邮</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -628,9 +694,6 @@
       <x:c r="M2" s="0" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="N2" s="0" t="n">
-        <x:v>1</x:v>
-      </x:c>
       <x:c r="O2" s="0" t="s">
         <x:v>28</x:v>
       </x:c>
@@ -705,25 +768,122 @@
         <x:v>47</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="I4" s="0" t="s">
+      <x:c r="J4" s="0" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="J4" s="0" t="s">
+      <x:c r="K4" s="0" t="s">
         <x:v>50</x:v>
       </x:c>
-      <x:c r="K4" s="0" t="s">
+      <x:c r="L4" s="0" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="L4" s="0" t="s">
+      <x:c r="M4" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="M4" s="0" t="s">
+      <x:c r="N4" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="O4" s="0" t="s">
         <x:v>53</x:v>
       </x:c>
-      <x:c r="O4" s="0" t="s">
+    </x:row>
+    <x:row r="5" spans="1:15">
+      <x:c r="A5" s="0" t="s">
         <x:v>54</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="G5" s="0" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="I5" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="K5" s="0" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="L5" s="0" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="M5" s="0" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="N5" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="O5" s="0" t="s">
+        <x:v>66</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:15">
+      <x:c r="A6" s="0" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="K6" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="L6" s="0" t="s">
+        <x:v>74</x:v>
+      </x:c>
+      <x:c r="M6" s="0" t="s">
+        <x:v>75</x:v>
+      </x:c>
+      <x:c r="N6" s="0" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="O6" s="0" t="s">
+        <x:v>76</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>